<commit_message>
Day 1 of flight trials.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2375BA5-EEDD-BE4B-8331-86C165F80FC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F53F48-B8A3-9047-9EA5-3BBF499A1537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23080" windowHeight="16620" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
+    <workbookView xWindow="5580" yWindow="500" windowWidth="26880" windowHeight="16720" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -108,7 +108,13 @@
     <t>Y</t>
   </si>
   <si>
-    <t>y</t>
+    <t>page</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -139,12 +145,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -256,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -268,6 +280,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322886B1-E7FD-B647-8810-B789824E1075}">
   <dimension ref="A1:Q445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,6 +673,9 @@
       <c r="P1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="Q1" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
@@ -685,7 +704,9 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="6"/>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
@@ -830,7 +851,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="8"/>
-      <c r="Q7" s="10"/>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
@@ -890,7 +911,7 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="10"/>
+      <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -919,7 +940,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="10"/>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
@@ -948,7 +969,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="8"/>
-      <c r="Q11" s="10"/>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
@@ -1064,7 +1085,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="10"/>
+      <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -1093,7 +1114,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="10"/>
+      <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -1122,7 +1143,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="8"/>
-      <c r="Q17" s="10"/>
+      <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -1151,7 +1172,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="8"/>
-      <c r="Q18" s="10"/>
+      <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
@@ -1180,7 +1201,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="8"/>
-      <c r="Q19" s="10"/>
+      <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
@@ -1209,7 +1230,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="8"/>
-      <c r="Q20" s="10"/>
+      <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -1238,7 +1259,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="8"/>
-      <c r="Q21" s="10"/>
+      <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -1267,7 +1288,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="8"/>
-      <c r="Q22" s="10"/>
+      <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -1325,7 +1346,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="8"/>
-      <c r="Q24" s="10"/>
+      <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
@@ -1354,7 +1375,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="8"/>
-      <c r="Q25" s="10"/>
+      <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -1383,7 +1404,7 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="8"/>
-      <c r="Q26" s="10"/>
+      <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
@@ -1441,7 +1462,7 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="8"/>
-      <c r="Q28" s="10"/>
+      <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
@@ -1499,7 +1520,7 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="8"/>
-      <c r="Q30" s="10"/>
+      <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
@@ -1637,6 +1658,9 @@
       <c r="P34" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="Q34">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
@@ -2587,6 +2611,9 @@
       <c r="P67" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="Q67">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
@@ -2615,6 +2642,9 @@
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
       <c r="P68" s="8"/>
+      <c r="Q68" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
@@ -2643,7 +2673,9 @@
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
       <c r="P69" s="8"/>
-      <c r="Q69" s="1"/>
+      <c r="Q69" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
@@ -2672,6 +2704,9 @@
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
       <c r="P70" s="6"/>
+      <c r="Q70" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
@@ -2700,34 +2735,40 @@
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
       <c r="P71" s="8"/>
+      <c r="Q71" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A72" s="7">
+      <c r="A72" s="12">
         <v>88</v>
       </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I72" s="5">
-        <v>70</v>
-      </c>
-      <c r="J72" s="7" t="s">
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="13">
+        <v>70</v>
+      </c>
+      <c r="J72" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K72" s="7"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7">
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12">
         <v>88</v>
       </c>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="8"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="14"/>
+      <c r="Q72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
@@ -2756,6 +2797,9 @@
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
       <c r="P73" s="8"/>
+      <c r="Q73" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -2784,6 +2828,9 @@
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
       <c r="P74" s="8"/>
+      <c r="Q74" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
@@ -2812,6 +2859,9 @@
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
       <c r="P75" s="8"/>
+      <c r="Q75" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
@@ -2840,6 +2890,9 @@
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
       <c r="P76" s="8"/>
+      <c r="Q76" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
@@ -2868,6 +2921,9 @@
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
       <c r="P77" s="8"/>
+      <c r="Q77" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
@@ -2896,6 +2952,9 @@
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
       <c r="P78" s="8"/>
+      <c r="Q78" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
@@ -2924,6 +2983,9 @@
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
       <c r="P79" s="8"/>
+      <c r="Q79" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
@@ -2952,8 +3014,11 @@
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
       <c r="P80" s="8"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>74</v>
       </c>
@@ -2980,8 +3045,11 @@
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
       <c r="P81" s="8"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>151</v>
       </c>
@@ -3008,8 +3076,11 @@
       <c r="N82" s="7"/>
       <c r="O82" s="7"/>
       <c r="P82" s="8"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q82" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>14</v>
       </c>
@@ -3036,8 +3107,11 @@
       <c r="N83" s="7"/>
       <c r="O83" s="7"/>
       <c r="P83" s="8"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q83" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>20</v>
       </c>
@@ -3064,8 +3138,11 @@
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
       <c r="P84" s="8"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q84" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>35</v>
       </c>
@@ -3092,8 +3169,11 @@
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
       <c r="P85" s="8"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q85" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>26</v>
       </c>
@@ -3120,8 +3200,11 @@
       <c r="N86" s="7"/>
       <c r="O86" s="7"/>
       <c r="P86" s="8"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q86" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>301</v>
       </c>
@@ -3148,8 +3231,11 @@
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
       <c r="P87" s="8"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>207</v>
       </c>
@@ -3176,8 +3262,11 @@
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
       <c r="P88" s="8"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>164</v>
       </c>
@@ -3204,8 +3293,11 @@
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
       <c r="P89" s="8"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>277</v>
       </c>
@@ -3232,8 +3324,11 @@
       <c r="N90" s="7"/>
       <c r="O90" s="7"/>
       <c r="P90" s="8"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>384</v>
       </c>
@@ -3260,8 +3355,11 @@
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
       <c r="P91" s="8"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q91" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>77</v>
       </c>
@@ -3290,8 +3388,11 @@
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
       <c r="P92" s="8"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q92" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>332</v>
       </c>
@@ -3318,8 +3419,11 @@
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
       <c r="P93" s="8"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>376</v>
       </c>
@@ -3346,8 +3450,11 @@
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
       <c r="P94" s="8"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q94" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>225</v>
       </c>
@@ -3374,8 +3481,11 @@
       <c r="N95" s="7"/>
       <c r="O95" s="7"/>
       <c r="P95" s="8"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>190</v>
       </c>
@@ -3402,6 +3512,9 @@
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
       <c r="P96" s="8"/>
+      <c r="Q96" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
@@ -3430,6 +3543,9 @@
       <c r="N97" s="7"/>
       <c r="O97" s="7"/>
       <c r="P97" s="8"/>
+      <c r="Q97" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -3458,6 +3574,9 @@
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
       <c r="P98" s="8"/>
+      <c r="Q98" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="99" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
@@ -3486,6 +3605,9 @@
       <c r="N99" s="7"/>
       <c r="O99" s="7"/>
       <c r="P99" s="8"/>
+      <c r="Q99" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="100" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
@@ -3535,6 +3657,9 @@
       </c>
       <c r="P100" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="Q100">
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
@@ -3592,12 +3717,17 @@
       <c r="N102" s="7"/>
       <c r="O102" s="7"/>
       <c r="P102" s="8"/>
+      <c r="Q102" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>100</v>
       </c>
-      <c r="B103" s="7"/>
+      <c r="B103" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
@@ -3620,7 +3750,9 @@
       <c r="N103" s="7"/>
       <c r="O103" s="7"/>
       <c r="P103" s="8"/>
-      <c r="Q103" s="1"/>
+      <c r="Q103" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
@@ -3649,6 +3781,9 @@
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
       <c r="P104" s="6"/>
+      <c r="Q104" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
@@ -3677,6 +3812,9 @@
       <c r="N105" s="7"/>
       <c r="O105" s="7"/>
       <c r="P105" s="8"/>
+      <c r="Q105" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
@@ -3705,6 +3843,9 @@
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
       <c r="P106" s="8"/>
+      <c r="Q106" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
@@ -3733,6 +3874,9 @@
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
       <c r="P107" s="8"/>
+      <c r="Q107" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
@@ -3761,6 +3905,9 @@
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
       <c r="P108" s="8"/>
+      <c r="Q108" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
@@ -3789,6 +3936,9 @@
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
       <c r="P109" s="8"/>
+      <c r="Q109" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -3817,34 +3967,40 @@
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
       <c r="P110" s="8"/>
+      <c r="Q110" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A111" s="7">
+      <c r="A111" s="12">
         <v>227</v>
       </c>
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I111" s="5">
-        <v>70</v>
-      </c>
-      <c r="J111" s="7" t="s">
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="H111" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I111" s="13">
+        <v>70</v>
+      </c>
+      <c r="J111" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K111" s="7"/>
-      <c r="L111" s="7"/>
-      <c r="M111" s="7">
+      <c r="K111" s="12"/>
+      <c r="L111" s="12"/>
+      <c r="M111" s="12">
         <v>227</v>
       </c>
-      <c r="N111" s="7"/>
-      <c r="O111" s="7"/>
-      <c r="P111" s="8"/>
+      <c r="N111" s="12"/>
+      <c r="O111" s="12"/>
+      <c r="P111" s="14"/>
+      <c r="Q111" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
@@ -3873,8 +4029,11 @@
       <c r="N112" s="7"/>
       <c r="O112" s="7"/>
       <c r="P112" s="8"/>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q112" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>182</v>
       </c>
@@ -3901,8 +4060,11 @@
       <c r="N113" s="7"/>
       <c r="O113" s="7"/>
       <c r="P113" s="8"/>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q113" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
         <v>313</v>
       </c>
@@ -3929,8 +4091,11 @@
       <c r="N114" s="7"/>
       <c r="O114" s="7"/>
       <c r="P114" s="8"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q114" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
         <v>361</v>
       </c>
@@ -3957,8 +4122,11 @@
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
       <c r="P115" s="8"/>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>177</v>
       </c>
@@ -3985,8 +4153,11 @@
       <c r="N116" s="7"/>
       <c r="O116" s="7"/>
       <c r="P116" s="8"/>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q116" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
         <v>180</v>
       </c>
@@ -4013,12 +4184,17 @@
       <c r="N117" s="7"/>
       <c r="O117" s="7"/>
       <c r="P117" s="8"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q117" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
         <v>91</v>
       </c>
-      <c r="B118" s="7"/>
+      <c r="B118" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
@@ -4041,8 +4217,11 @@
       <c r="N118" s="7"/>
       <c r="O118" s="7"/>
       <c r="P118" s="8"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q118" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
         <v>41</v>
       </c>
@@ -4069,8 +4248,11 @@
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
       <c r="P119" s="8"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q119" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>174</v>
       </c>
@@ -4097,8 +4279,11 @@
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
       <c r="P120" s="8"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q120" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>39</v>
       </c>
@@ -4125,8 +4310,11 @@
       <c r="N121" s="7"/>
       <c r="O121" s="7"/>
       <c r="P121" s="8"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q121" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>186</v>
       </c>
@@ -4153,8 +4341,11 @@
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
       <c r="P122" s="8"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q122" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>60</v>
       </c>
@@ -4181,8 +4372,11 @@
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
       <c r="P123" s="8"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q123" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>262</v>
       </c>
@@ -4209,8 +4403,11 @@
       <c r="N124" s="7"/>
       <c r="O124" s="7"/>
       <c r="P124" s="8"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q124" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>245</v>
       </c>
@@ -4237,8 +4434,11 @@
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
       <c r="P125" s="8"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q125" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
         <v>345</v>
       </c>
@@ -4265,8 +4465,11 @@
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
       <c r="P126" s="8"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q126" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
         <v>79</v>
       </c>
@@ -4293,8 +4496,11 @@
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
       <c r="P127" s="8"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q127" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
         <v>66</v>
       </c>
@@ -4321,13 +4527,16 @@
       <c r="N128" s="7"/>
       <c r="O128" s="7"/>
       <c r="P128" s="8"/>
+      <c r="Q128" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
         <v>289</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
@@ -4351,6 +4560,9 @@
       <c r="N129" s="7"/>
       <c r="O129" s="7"/>
       <c r="P129" s="8"/>
+      <c r="Q129" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
@@ -4379,6 +4591,9 @@
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
       <c r="P130" s="8"/>
+      <c r="Q130" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
@@ -4407,34 +4622,40 @@
       <c r="N131" s="7"/>
       <c r="O131" s="7"/>
       <c r="P131" s="8"/>
+      <c r="Q131" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="132" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="7">
+      <c r="A132" s="12">
         <v>162</v>
       </c>
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="7"/>
-      <c r="G132" s="7"/>
-      <c r="H132" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I132" s="5">
-        <v>70</v>
-      </c>
-      <c r="J132" s="7" t="s">
+      <c r="B132" s="12"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
+      <c r="H132" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I132" s="13">
+        <v>70</v>
+      </c>
+      <c r="J132" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K132" s="7"/>
-      <c r="L132" s="7"/>
-      <c r="M132" s="7">
+      <c r="K132" s="12"/>
+      <c r="L132" s="12"/>
+      <c r="M132" s="12">
         <v>162</v>
       </c>
-      <c r="N132" s="7"/>
-      <c r="O132" s="7"/>
-      <c r="P132" s="8"/>
+      <c r="N132" s="12"/>
+      <c r="O132" s="12"/>
+      <c r="P132" s="14"/>
+      <c r="Q132" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="133" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
@@ -4518,7 +4739,9 @@
       <c r="A135" s="7">
         <v>115</v>
       </c>
-      <c r="B135" s="7"/>
+      <c r="B135" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="7"/>
@@ -7363,7 +7586,9 @@
       <c r="A234" s="7">
         <v>199</v>
       </c>
-      <c r="B234" s="7"/>
+      <c r="B234" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C234" s="7"/>
       <c r="D234" s="7"/>
       <c r="E234" s="7"/>
@@ -7840,7 +8065,9 @@
       <c r="A251" s="7">
         <v>273</v>
       </c>
-      <c r="B251" s="7"/>
+      <c r="B251" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C251" s="7"/>
       <c r="D251" s="7"/>
       <c r="E251" s="7"/>
@@ -7924,7 +8151,9 @@
       <c r="A254" s="7">
         <v>95</v>
       </c>
-      <c r="B254" s="7"/>
+      <c r="B254" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C254" s="7"/>
       <c r="D254" s="7"/>
       <c r="E254" s="7"/>
@@ -8759,7 +8988,9 @@
       <c r="A283" s="7">
         <v>21</v>
       </c>
-      <c r="B283" s="7"/>
+      <c r="B283" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C283" s="7"/>
       <c r="D283" s="7"/>
       <c r="E283" s="7"/>
@@ -8927,7 +9158,9 @@
       <c r="A289" s="7">
         <v>261</v>
       </c>
-      <c r="B289" s="7"/>
+      <c r="B289" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C289" s="7"/>
       <c r="D289" s="7"/>
       <c r="E289" s="7"/>
@@ -9960,7 +10193,9 @@
       <c r="A325" s="7">
         <v>6</v>
       </c>
-      <c r="B325" s="7"/>
+      <c r="B325" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C325" s="7"/>
       <c r="D325" s="7"/>
       <c r="E325" s="7"/>
@@ -11353,7 +11588,9 @@
       <c r="A373" s="7">
         <v>386</v>
       </c>
-      <c r="B373" s="7"/>
+      <c r="B373" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C373" s="7"/>
       <c r="D373" s="7"/>
       <c r="E373" s="7"/>
@@ -11438,7 +11675,9 @@
       <c r="A376" s="7">
         <v>163</v>
       </c>
-      <c r="B376" s="5"/>
+      <c r="B376" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="C376" s="5"/>
       <c r="D376" s="5"/>
       <c r="E376" s="5"/>
@@ -11802,7 +12041,9 @@
       <c r="A389" s="7">
         <v>266</v>
       </c>
-      <c r="B389" s="7"/>
+      <c r="B389" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C389" s="7"/>
       <c r="D389" s="7"/>
       <c r="E389" s="7"/>
@@ -12246,7 +12487,9 @@
       <c r="A404" s="7">
         <v>80</v>
       </c>
-      <c r="B404" s="7"/>
+      <c r="B404" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
       <c r="E404" s="7"/>
@@ -12386,7 +12629,9 @@
       <c r="A409" s="7">
         <v>390</v>
       </c>
-      <c r="B409" s="7"/>
+      <c r="B409" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C409" s="7"/>
       <c r="D409" s="7"/>
       <c r="E409" s="7"/>
@@ -12415,7 +12660,9 @@
       <c r="A410" s="7">
         <v>167</v>
       </c>
-      <c r="B410" s="5"/>
+      <c r="B410" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="C410" s="5"/>
       <c r="D410" s="5"/>
       <c r="E410" s="5"/>
@@ -12471,7 +12718,9 @@
       <c r="A412" s="7">
         <v>279</v>
       </c>
-      <c r="B412" s="7"/>
+      <c r="B412" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C412" s="7"/>
       <c r="D412" s="7"/>
       <c r="E412" s="7"/>

</xml_diff>

<commit_message>
Added dead bugs of the day.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F53F48-B8A3-9047-9EA5-3BBF499A1537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF615267-B357-BB4A-BE3A-98F45F62E7DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="500" windowWidth="26880" windowHeight="16720" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
+    <workbookView xWindow="2120" yWindow="500" windowWidth="26880" windowHeight="16640" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322886B1-E7FD-B647-8810-B789824E1075}">
   <dimension ref="A1:Q445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4161,7 +4161,9 @@
       <c r="A117" s="7">
         <v>180</v>
       </c>
-      <c r="B117" s="7"/>
+      <c r="B117" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
@@ -5803,7 +5805,9 @@
       <c r="A172" s="7">
         <v>379</v>
       </c>
-      <c r="B172" s="5"/>
+      <c r="B172" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
       <c r="E172" s="5"/>
@@ -6637,7 +6641,9 @@
       <c r="A201" s="7">
         <v>30</v>
       </c>
-      <c r="B201" s="7"/>
+      <c r="B201" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C201" s="7"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
@@ -7396,7 +7402,9 @@
       <c r="A228" s="7">
         <v>13</v>
       </c>
-      <c r="B228" s="7"/>
+      <c r="B228" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C228" s="7"/>
       <c r="D228" s="7"/>
       <c r="E228" s="7"/>
@@ -8349,7 +8357,9 @@
       <c r="A261" s="7">
         <v>40</v>
       </c>
-      <c r="B261" s="7"/>
+      <c r="B261" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C261" s="7"/>
       <c r="D261" s="7"/>
       <c r="E261" s="7"/>
@@ -11146,7 +11156,9 @@
       <c r="A358" s="7">
         <v>87</v>
       </c>
-      <c r="B358" s="7"/>
+      <c r="B358" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C358" s="7"/>
       <c r="D358" s="7"/>
       <c r="E358" s="7"/>
@@ -11174,7 +11186,9 @@
       <c r="A359" s="7">
         <v>219</v>
       </c>
-      <c r="B359" s="7"/>
+      <c r="B359" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C359" s="7"/>
       <c r="D359" s="7"/>
       <c r="E359" s="7"/>
@@ -12545,7 +12559,9 @@
       <c r="A406" s="7">
         <v>366</v>
       </c>
-      <c r="B406" s="7"/>
+      <c r="B406" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C406" s="7"/>
       <c r="D406" s="7"/>
       <c r="E406" s="7"/>

</xml_diff>

<commit_message>
Flight trial prep day 2.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF615267-B357-BB4A-BE3A-98F45F62E7DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C26E6B-89BC-C742-B3EA-3C1F7B0AE786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="500" windowWidth="26880" windowHeight="16640" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -114,7 +114,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>?</t>
+    <t>already tested</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="A1:Q445"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A176" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+      <selection activeCell="Q198" sqref="Q198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2642,9 +2642,6 @@
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
       <c r="P68" s="8"/>
-      <c r="Q68" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
@@ -2673,9 +2670,7 @@
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
       <c r="P69" s="8"/>
-      <c r="Q69" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q69" s="1"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
@@ -2704,9 +2699,6 @@
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
       <c r="P70" s="6"/>
-      <c r="Q70" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
@@ -2735,9 +2727,6 @@
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
       <c r="P71" s="8"/>
-      <c r="Q71" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="12">
@@ -2767,7 +2756,7 @@
       <c r="O72" s="12"/>
       <c r="P72" s="14"/>
       <c r="Q72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
@@ -2797,9 +2786,6 @@
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
       <c r="P73" s="8"/>
-      <c r="Q73" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -2828,9 +2814,6 @@
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
       <c r="P74" s="8"/>
-      <c r="Q74" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
@@ -2859,9 +2842,6 @@
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
       <c r="P75" s="8"/>
-      <c r="Q75" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
@@ -2890,9 +2870,6 @@
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
       <c r="P76" s="8"/>
-      <c r="Q76" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
@@ -2921,9 +2898,6 @@
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
       <c r="P77" s="8"/>
-      <c r="Q77" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
@@ -2952,9 +2926,6 @@
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
       <c r="P78" s="8"/>
-      <c r="Q78" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
@@ -2983,9 +2954,6 @@
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
       <c r="P79" s="8"/>
-      <c r="Q79" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
@@ -3014,11 +2982,8 @@
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
       <c r="P80" s="8"/>
-      <c r="Q80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>74</v>
       </c>
@@ -3045,11 +3010,8 @@
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
       <c r="P81" s="8"/>
-      <c r="Q81" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>151</v>
       </c>
@@ -3076,11 +3038,8 @@
       <c r="N82" s="7"/>
       <c r="O82" s="7"/>
       <c r="P82" s="8"/>
-      <c r="Q82" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>14</v>
       </c>
@@ -3107,11 +3066,8 @@
       <c r="N83" s="7"/>
       <c r="O83" s="7"/>
       <c r="P83" s="8"/>
-      <c r="Q83" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>20</v>
       </c>
@@ -3138,11 +3094,8 @@
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
       <c r="P84" s="8"/>
-      <c r="Q84" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>35</v>
       </c>
@@ -3169,11 +3122,8 @@
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
       <c r="P85" s="8"/>
-      <c r="Q85" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>26</v>
       </c>
@@ -3200,11 +3150,8 @@
       <c r="N86" s="7"/>
       <c r="O86" s="7"/>
       <c r="P86" s="8"/>
-      <c r="Q86" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>301</v>
       </c>
@@ -3231,11 +3178,8 @@
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
       <c r="P87" s="8"/>
-      <c r="Q87" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>207</v>
       </c>
@@ -3262,11 +3206,8 @@
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
       <c r="P88" s="8"/>
-      <c r="Q88" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>164</v>
       </c>
@@ -3293,11 +3234,8 @@
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
       <c r="P89" s="8"/>
-      <c r="Q89" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>277</v>
       </c>
@@ -3324,11 +3262,8 @@
       <c r="N90" s="7"/>
       <c r="O90" s="7"/>
       <c r="P90" s="8"/>
-      <c r="Q90" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>384</v>
       </c>
@@ -3355,11 +3290,8 @@
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
       <c r="P91" s="8"/>
-      <c r="Q91" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>77</v>
       </c>
@@ -3388,11 +3320,8 @@
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
       <c r="P92" s="8"/>
-      <c r="Q92" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>332</v>
       </c>
@@ -3419,11 +3348,8 @@
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
       <c r="P93" s="8"/>
-      <c r="Q93" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>376</v>
       </c>
@@ -3450,11 +3376,8 @@
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
       <c r="P94" s="8"/>
-      <c r="Q94" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>225</v>
       </c>
@@ -3481,11 +3404,8 @@
       <c r="N95" s="7"/>
       <c r="O95" s="7"/>
       <c r="P95" s="8"/>
-      <c r="Q95" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>190</v>
       </c>
@@ -3512,9 +3432,6 @@
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
       <c r="P96" s="8"/>
-      <c r="Q96" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
@@ -3543,9 +3460,6 @@
       <c r="N97" s="7"/>
       <c r="O97" s="7"/>
       <c r="P97" s="8"/>
-      <c r="Q97" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -3574,9 +3488,6 @@
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
       <c r="P98" s="8"/>
-      <c r="Q98" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="99" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
@@ -3605,9 +3516,6 @@
       <c r="N99" s="7"/>
       <c r="O99" s="7"/>
       <c r="P99" s="8"/>
-      <c r="Q99" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="100" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
@@ -3717,9 +3625,6 @@
       <c r="N102" s="7"/>
       <c r="O102" s="7"/>
       <c r="P102" s="8"/>
-      <c r="Q102" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
@@ -3750,9 +3655,7 @@
       <c r="N103" s="7"/>
       <c r="O103" s="7"/>
       <c r="P103" s="8"/>
-      <c r="Q103" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q103" s="1"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
@@ -3781,9 +3684,7 @@
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
       <c r="P104" s="6"/>
-      <c r="Q104" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q104" s="10"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
@@ -3812,9 +3713,6 @@
       <c r="N105" s="7"/>
       <c r="O105" s="7"/>
       <c r="P105" s="8"/>
-      <c r="Q105" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
@@ -3843,9 +3741,6 @@
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
       <c r="P106" s="8"/>
-      <c r="Q106" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
@@ -3874,9 +3769,6 @@
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
       <c r="P107" s="8"/>
-      <c r="Q107" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
@@ -3905,9 +3797,6 @@
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
       <c r="P108" s="8"/>
-      <c r="Q108" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
@@ -3936,9 +3825,6 @@
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
       <c r="P109" s="8"/>
-      <c r="Q109" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -3967,9 +3853,6 @@
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
       <c r="P110" s="8"/>
-      <c r="Q110" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="12">
@@ -3999,7 +3882,7 @@
       <c r="O111" s="12"/>
       <c r="P111" s="14"/>
       <c r="Q111" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
@@ -4029,9 +3912,6 @@
       <c r="N112" s="7"/>
       <c r="O112" s="7"/>
       <c r="P112" s="8"/>
-      <c r="Q112" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
@@ -4060,37 +3940,34 @@
       <c r="N113" s="7"/>
       <c r="O113" s="7"/>
       <c r="P113" s="8"/>
-      <c r="Q113" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A114" s="7">
+      <c r="A114" s="12">
         <v>313</v>
       </c>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
-      <c r="G114" s="7"/>
-      <c r="H114" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I114" s="5">
-        <v>70</v>
-      </c>
-      <c r="J114" s="7" t="s">
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+      <c r="H114" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I114" s="13">
+        <v>70</v>
+      </c>
+      <c r="J114" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K114" s="7"/>
-      <c r="L114" s="7"/>
-      <c r="M114" s="7">
+      <c r="K114" s="12"/>
+      <c r="L114" s="12"/>
+      <c r="M114" s="12">
         <v>313</v>
       </c>
-      <c r="N114" s="7"/>
-      <c r="O114" s="7"/>
-      <c r="P114" s="8"/>
+      <c r="N114" s="12"/>
+      <c r="O114" s="12"/>
+      <c r="P114" s="14"/>
       <c r="Q114" t="s">
         <v>28</v>
       </c>
@@ -4122,9 +3999,6 @@
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
       <c r="P115" s="8"/>
-      <c r="Q115" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
@@ -4153,9 +4027,6 @@
       <c r="N116" s="7"/>
       <c r="O116" s="7"/>
       <c r="P116" s="8"/>
-      <c r="Q116" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
@@ -4186,9 +4057,6 @@
       <c r="N117" s="7"/>
       <c r="O117" s="7"/>
       <c r="P117" s="8"/>
-      <c r="Q117" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
@@ -4219,9 +4087,6 @@
       <c r="N118" s="7"/>
       <c r="O118" s="7"/>
       <c r="P118" s="8"/>
-      <c r="Q118" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
@@ -4250,9 +4115,6 @@
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
       <c r="P119" s="8"/>
-      <c r="Q119" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
@@ -4281,9 +4143,6 @@
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
       <c r="P120" s="8"/>
-      <c r="Q120" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
@@ -4312,9 +4171,6 @@
       <c r="N121" s="7"/>
       <c r="O121" s="7"/>
       <c r="P121" s="8"/>
-      <c r="Q121" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
@@ -4343,9 +4199,6 @@
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
       <c r="P122" s="8"/>
-      <c r="Q122" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
@@ -4374,9 +4227,6 @@
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
       <c r="P123" s="8"/>
-      <c r="Q123" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
@@ -4405,9 +4255,6 @@
       <c r="N124" s="7"/>
       <c r="O124" s="7"/>
       <c r="P124" s="8"/>
-      <c r="Q124" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
@@ -4436,9 +4283,6 @@
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
       <c r="P125" s="8"/>
-      <c r="Q125" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
@@ -4467,9 +4311,6 @@
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
       <c r="P126" s="8"/>
-      <c r="Q126" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
@@ -4498,9 +4339,6 @@
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
       <c r="P127" s="8"/>
-      <c r="Q127" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
@@ -4529,9 +4367,6 @@
       <c r="N128" s="7"/>
       <c r="O128" s="7"/>
       <c r="P128" s="8"/>
-      <c r="Q128" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
@@ -4562,9 +4397,6 @@
       <c r="N129" s="7"/>
       <c r="O129" s="7"/>
       <c r="P129" s="8"/>
-      <c r="Q129" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
@@ -4593,9 +4425,6 @@
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
       <c r="P130" s="8"/>
-      <c r="Q130" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
@@ -4624,9 +4453,6 @@
       <c r="N131" s="7"/>
       <c r="O131" s="7"/>
       <c r="P131" s="8"/>
-      <c r="Q131" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="132" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12">
@@ -4655,9 +4481,6 @@
       <c r="N132" s="12"/>
       <c r="O132" s="12"/>
       <c r="P132" s="14"/>
-      <c r="Q132" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="133" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
@@ -4707,6 +4530,9 @@
       </c>
       <c r="P133" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="Q133">
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
@@ -4736,6 +4562,9 @@
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
       <c r="P134" s="8"/>
+      <c r="Q134" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
@@ -4766,6 +4595,9 @@
       <c r="N135" s="7"/>
       <c r="O135" s="7"/>
       <c r="P135" s="8"/>
+      <c r="Q135" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
@@ -4794,6 +4626,9 @@
       <c r="N136" s="7"/>
       <c r="O136" s="7"/>
       <c r="P136" s="8"/>
+      <c r="Q136" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
@@ -4822,7 +4657,9 @@
       <c r="N137" s="7"/>
       <c r="O137" s="7"/>
       <c r="P137" s="8"/>
-      <c r="Q137" s="1"/>
+      <c r="Q137" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
@@ -4851,6 +4688,9 @@
       <c r="N138" s="5"/>
       <c r="O138" s="5"/>
       <c r="P138" s="6"/>
+      <c r="Q138" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
@@ -4879,6 +4719,9 @@
       <c r="N139" s="7"/>
       <c r="O139" s="7"/>
       <c r="P139" s="8"/>
+      <c r="Q139" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
@@ -4907,6 +4750,9 @@
       <c r="N140" s="7"/>
       <c r="O140" s="7"/>
       <c r="P140" s="8"/>
+      <c r="Q140" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
@@ -4935,6 +4781,9 @@
       <c r="N141" s="7"/>
       <c r="O141" s="7"/>
       <c r="P141" s="8"/>
+      <c r="Q141" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
@@ -4963,6 +4812,9 @@
       <c r="N142" s="7"/>
       <c r="O142" s="7"/>
       <c r="P142" s="8"/>
+      <c r="Q142" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
@@ -4991,6 +4843,9 @@
       <c r="N143" s="7"/>
       <c r="O143" s="7"/>
       <c r="P143" s="8"/>
+      <c r="Q143" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
@@ -5019,8 +4874,11 @@
       <c r="N144" s="7"/>
       <c r="O144" s="7"/>
       <c r="P144" s="8"/>
-    </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q144" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
         <v>82</v>
       </c>
@@ -5049,8 +4907,11 @@
       <c r="N145" s="7"/>
       <c r="O145" s="7"/>
       <c r="P145" s="8"/>
-    </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q145" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
         <v>293</v>
       </c>
@@ -5077,8 +4938,11 @@
       <c r="N146" s="7"/>
       <c r="O146" s="7"/>
       <c r="P146" s="8"/>
-    </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q146" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
         <v>348</v>
       </c>
@@ -5105,8 +4969,11 @@
       <c r="N147" s="7"/>
       <c r="O147" s="7"/>
       <c r="P147" s="8"/>
-    </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q147" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
         <v>169</v>
       </c>
@@ -5133,8 +5000,11 @@
       <c r="N148" s="7"/>
       <c r="O148" s="7"/>
       <c r="P148" s="8"/>
-    </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q148" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
         <v>365</v>
       </c>
@@ -5161,8 +5031,11 @@
       <c r="N149" s="7"/>
       <c r="O149" s="7"/>
       <c r="P149" s="8"/>
-    </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q149" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
         <v>116</v>
       </c>
@@ -5189,8 +5062,11 @@
       <c r="N150" s="7"/>
       <c r="O150" s="7"/>
       <c r="P150" s="8"/>
-    </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q150" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
         <v>54</v>
       </c>
@@ -5217,8 +5093,11 @@
       <c r="N151" s="7"/>
       <c r="O151" s="7"/>
       <c r="P151" s="8"/>
-    </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q151" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
         <v>359</v>
       </c>
@@ -5245,8 +5124,11 @@
       <c r="N152" s="7"/>
       <c r="O152" s="7"/>
       <c r="P152" s="8"/>
-    </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q152" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
         <v>194</v>
       </c>
@@ -5273,8 +5155,11 @@
       <c r="N153" s="7"/>
       <c r="O153" s="7"/>
       <c r="P153" s="8"/>
-    </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q153" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
         <v>58</v>
       </c>
@@ -5301,8 +5186,11 @@
       <c r="N154" s="7"/>
       <c r="O154" s="7"/>
       <c r="P154" s="8"/>
-    </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q154" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
         <v>7</v>
       </c>
@@ -5329,8 +5217,11 @@
       <c r="N155" s="7"/>
       <c r="O155" s="7"/>
       <c r="P155" s="8"/>
-    </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q155" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>129</v>
       </c>
@@ -5357,8 +5248,11 @@
       <c r="N156" s="7"/>
       <c r="O156" s="7"/>
       <c r="P156" s="8"/>
-    </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q156" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
         <v>119</v>
       </c>
@@ -5385,8 +5279,11 @@
       <c r="N157" s="7"/>
       <c r="O157" s="7"/>
       <c r="P157" s="8"/>
-    </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q157" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
         <v>249</v>
       </c>
@@ -5413,8 +5310,11 @@
       <c r="N158" s="7"/>
       <c r="O158" s="7"/>
       <c r="P158" s="8"/>
-    </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q158" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
         <v>36</v>
       </c>
@@ -5441,8 +5341,11 @@
       <c r="N159" s="7"/>
       <c r="O159" s="7"/>
       <c r="P159" s="8"/>
-    </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q159" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
         <v>175</v>
       </c>
@@ -5469,6 +5372,9 @@
       <c r="N160" s="7"/>
       <c r="O160" s="7"/>
       <c r="P160" s="8"/>
+      <c r="Q160" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
@@ -5497,6 +5403,9 @@
       <c r="N161" s="7"/>
       <c r="O161" s="7"/>
       <c r="P161" s="8"/>
+      <c r="Q161" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
@@ -5525,6 +5434,9 @@
       <c r="N162" s="7"/>
       <c r="O162" s="7"/>
       <c r="P162" s="8"/>
+      <c r="Q162" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
@@ -5553,6 +5465,9 @@
       <c r="N163" s="7"/>
       <c r="O163" s="7"/>
       <c r="P163" s="8"/>
+      <c r="Q163" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
@@ -5581,6 +5496,9 @@
       <c r="N164" s="7"/>
       <c r="O164" s="7"/>
       <c r="P164" s="8"/>
+      <c r="Q164" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="165" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7">
@@ -5609,6 +5527,9 @@
       <c r="N165" s="7"/>
       <c r="O165" s="7"/>
       <c r="P165" s="8"/>
+      <c r="Q165" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="166" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
@@ -5658,6 +5579,9 @@
       </c>
       <c r="P166" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="Q166">
+        <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
@@ -5687,6 +5611,9 @@
       <c r="N167" s="7"/>
       <c r="O167" s="7"/>
       <c r="P167" s="8"/>
+      <c r="Q167" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
@@ -5715,6 +5642,9 @@
       <c r="N168" s="7"/>
       <c r="O168" s="7"/>
       <c r="P168" s="8"/>
+      <c r="Q168" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
@@ -5743,6 +5673,9 @@
       <c r="N169" s="7"/>
       <c r="O169" s="7"/>
       <c r="P169" s="8"/>
+      <c r="Q169" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
@@ -5771,6 +5704,9 @@
       <c r="N170" s="7"/>
       <c r="O170" s="7"/>
       <c r="P170" s="8"/>
+      <c r="Q170" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
@@ -5799,7 +5735,9 @@
       <c r="N171" s="7"/>
       <c r="O171" s="7"/>
       <c r="P171" s="8"/>
-      <c r="Q171" s="1"/>
+      <c r="Q171" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
@@ -5830,6 +5768,9 @@
       <c r="N172" s="5"/>
       <c r="O172" s="5"/>
       <c r="P172" s="6"/>
+      <c r="Q172" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
@@ -5858,6 +5799,9 @@
       <c r="N173" s="7"/>
       <c r="O173" s="7"/>
       <c r="P173" s="8"/>
+      <c r="Q173" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
@@ -5886,6 +5830,9 @@
       <c r="N174" s="7"/>
       <c r="O174" s="7"/>
       <c r="P174" s="8"/>
+      <c r="Q174" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
@@ -5914,6 +5861,9 @@
       <c r="N175" s="7"/>
       <c r="O175" s="7"/>
       <c r="P175" s="8"/>
+      <c r="Q175" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
@@ -5942,8 +5892,11 @@
       <c r="N176" s="7"/>
       <c r="O176" s="7"/>
       <c r="P176" s="8"/>
-    </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q176" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
         <v>202</v>
       </c>
@@ -5970,36 +5923,42 @@
       <c r="N177" s="7"/>
       <c r="O177" s="7"/>
       <c r="P177" s="8"/>
-    </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A178" s="7">
+      <c r="Q177" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A178" s="12">
         <v>353</v>
       </c>
-      <c r="B178" s="7"/>
-      <c r="C178" s="7"/>
-      <c r="D178" s="7"/>
-      <c r="E178" s="7"/>
-      <c r="F178" s="7"/>
-      <c r="G178" s="7"/>
-      <c r="H178" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I178" s="5">
-        <v>70</v>
-      </c>
-      <c r="J178" s="7" t="s">
+      <c r="B178" s="12"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="12"/>
+      <c r="E178" s="12"/>
+      <c r="F178" s="12"/>
+      <c r="G178" s="12"/>
+      <c r="H178" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I178" s="13">
+        <v>70</v>
+      </c>
+      <c r="J178" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K178" s="7"/>
-      <c r="L178" s="7"/>
-      <c r="M178" s="7">
+      <c r="K178" s="12"/>
+      <c r="L178" s="12"/>
+      <c r="M178" s="12">
         <v>353</v>
       </c>
-      <c r="N178" s="7"/>
-      <c r="O178" s="7"/>
-      <c r="P178" s="8"/>
-    </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N178" s="12"/>
+      <c r="O178" s="12"/>
+      <c r="P178" s="14"/>
+      <c r="Q178" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
         <v>391</v>
       </c>
@@ -6026,8 +5985,11 @@
       <c r="N179" s="7"/>
       <c r="O179" s="7"/>
       <c r="P179" s="8"/>
-    </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q179" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
         <v>398</v>
       </c>
@@ -6054,8 +6016,11 @@
       <c r="N180" s="7"/>
       <c r="O180" s="7"/>
       <c r="P180" s="8"/>
-    </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q180" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
         <v>397</v>
       </c>
@@ -6082,8 +6047,11 @@
       <c r="N181" s="7"/>
       <c r="O181" s="7"/>
       <c r="P181" s="8"/>
-    </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q181" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" s="7">
         <v>258</v>
       </c>
@@ -6110,8 +6078,11 @@
       <c r="N182" s="7"/>
       <c r="O182" s="7"/>
       <c r="P182" s="8"/>
-    </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q182" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" s="7">
         <v>275</v>
       </c>
@@ -6138,8 +6109,11 @@
       <c r="N183" s="7"/>
       <c r="O183" s="7"/>
       <c r="P183" s="8"/>
-    </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q183" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
         <v>236</v>
       </c>
@@ -6166,8 +6140,11 @@
       <c r="N184" s="7"/>
       <c r="O184" s="7"/>
       <c r="P184" s="8"/>
-    </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q184" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
         <v>246</v>
       </c>
@@ -6194,8 +6171,11 @@
       <c r="N185" s="7"/>
       <c r="O185" s="7"/>
       <c r="P185" s="8"/>
-    </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q185" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
         <v>324</v>
       </c>
@@ -6222,8 +6202,11 @@
       <c r="N186" s="7"/>
       <c r="O186" s="7"/>
       <c r="P186" s="8"/>
-    </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q186" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
         <v>375</v>
       </c>
@@ -6250,8 +6233,11 @@
       <c r="N187" s="7"/>
       <c r="O187" s="7"/>
       <c r="P187" s="8"/>
-    </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q187" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
         <v>303</v>
       </c>
@@ -6278,8 +6264,11 @@
       <c r="N188" s="7"/>
       <c r="O188" s="7"/>
       <c r="P188" s="8"/>
-    </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q188" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
         <v>16</v>
       </c>
@@ -6306,8 +6295,11 @@
       <c r="N189" s="7"/>
       <c r="O189" s="7"/>
       <c r="P189" s="8"/>
-    </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q189" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
         <v>143</v>
       </c>
@@ -6334,8 +6326,11 @@
       <c r="N190" s="7"/>
       <c r="O190" s="7"/>
       <c r="P190" s="8"/>
-    </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q190" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
         <v>64</v>
       </c>
@@ -6362,8 +6357,11 @@
       <c r="N191" s="7"/>
       <c r="O191" s="7"/>
       <c r="P191" s="8"/>
-    </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q191" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" s="7">
         <v>55</v>
       </c>
@@ -6390,6 +6388,9 @@
       <c r="N192" s="7"/>
       <c r="O192" s="7"/>
       <c r="P192" s="8"/>
+      <c r="Q192" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" s="7">
@@ -6418,6 +6419,9 @@
       <c r="N193" s="7"/>
       <c r="O193" s="7"/>
       <c r="P193" s="8"/>
+      <c r="Q193" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" s="7">
@@ -6446,6 +6450,9 @@
       <c r="N194" s="7"/>
       <c r="O194" s="7"/>
       <c r="P194" s="8"/>
+      <c r="Q194" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
@@ -6474,6 +6481,9 @@
       <c r="N195" s="7"/>
       <c r="O195" s="7"/>
       <c r="P195" s="8"/>
+      <c r="Q195" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" s="7">
@@ -6502,6 +6512,9 @@
       <c r="N196" s="7"/>
       <c r="O196" s="7"/>
       <c r="P196" s="8"/>
+      <c r="Q196" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" s="7">
@@ -6530,6 +6543,9 @@
       <c r="N197" s="7"/>
       <c r="O197" s="7"/>
       <c r="P197" s="8"/>
+      <c r="Q197" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="198" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="7">
@@ -6558,6 +6574,9 @@
       <c r="N198" s="7"/>
       <c r="O198" s="7"/>
       <c r="P198" s="8"/>
+      <c r="Q198" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="199" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
@@ -6607,6 +6626,9 @@
       </c>
       <c r="P199" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="Q199">
+        <v>7</v>
       </c>
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.2">
@@ -7561,6 +7583,9 @@
       <c r="P232" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="Q232">
+        <v>8</v>
+      </c>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" s="7">
@@ -8241,7 +8266,7 @@
       <c r="O256" s="7"/>
       <c r="P256" s="8"/>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A257" s="7">
         <v>389</v>
       </c>
@@ -8269,7 +8294,7 @@
       <c r="O257" s="7"/>
       <c r="P257" s="8"/>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A258" s="7">
         <v>76</v>
       </c>
@@ -8297,7 +8322,7 @@
       <c r="O258" s="7"/>
       <c r="P258" s="8"/>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
         <v>285</v>
       </c>
@@ -8325,7 +8350,7 @@
       <c r="O259" s="7"/>
       <c r="P259" s="8"/>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A260" s="7">
         <v>233</v>
       </c>
@@ -8353,7 +8378,7 @@
       <c r="O260" s="7"/>
       <c r="P260" s="8"/>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" s="7">
         <v>40</v>
       </c>
@@ -8383,7 +8408,7 @@
       <c r="O261" s="7"/>
       <c r="P261" s="8"/>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A262" s="7">
         <v>42</v>
       </c>
@@ -8411,7 +8436,7 @@
       <c r="O262" s="7"/>
       <c r="P262" s="8"/>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" s="7">
         <v>240</v>
       </c>
@@ -8439,7 +8464,7 @@
       <c r="O263" s="7"/>
       <c r="P263" s="8"/>
     </row>
-    <row r="264" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A264" s="7">
         <v>213</v>
       </c>
@@ -8467,7 +8492,7 @@
       <c r="O264" s="7"/>
       <c r="P264" s="8"/>
     </row>
-    <row r="265" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>0</v>
       </c>
@@ -8516,8 +8541,11 @@
       <c r="P265" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q265">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A266" s="7">
         <v>184</v>
       </c>
@@ -8545,7 +8573,7 @@
       <c r="O266" s="7"/>
       <c r="P266" s="8"/>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A267" s="7">
         <v>117</v>
       </c>
@@ -8573,7 +8601,7 @@
       <c r="O267" s="7"/>
       <c r="P267" s="8"/>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A268" s="7">
         <v>238</v>
       </c>
@@ -8601,7 +8629,7 @@
       <c r="O268" s="7"/>
       <c r="P268" s="8"/>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A269" s="7">
         <v>181</v>
       </c>
@@ -8629,7 +8657,7 @@
       <c r="O269" s="7"/>
       <c r="P269" s="8"/>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A270" s="7">
         <v>314</v>
       </c>
@@ -8657,7 +8685,7 @@
       <c r="O270" s="7"/>
       <c r="P270" s="8"/>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A271" s="7">
         <v>83</v>
       </c>
@@ -8685,7 +8713,7 @@
       <c r="O271" s="7"/>
       <c r="P271" s="8"/>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A272" s="7">
         <v>195</v>
       </c>
@@ -9164,7 +9192,7 @@
       <c r="O288" s="7"/>
       <c r="P288" s="8"/>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A289" s="7">
         <v>261</v>
       </c>
@@ -9194,7 +9222,7 @@
       <c r="O289" s="7"/>
       <c r="P289" s="8"/>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A290" s="7">
         <v>244</v>
       </c>
@@ -9222,7 +9250,7 @@
       <c r="O290" s="7"/>
       <c r="P290" s="8"/>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" s="7">
         <v>171</v>
       </c>
@@ -9250,7 +9278,7 @@
       <c r="O291" s="7"/>
       <c r="P291" s="8"/>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A292" s="7">
         <v>352</v>
       </c>
@@ -9278,7 +9306,7 @@
       <c r="O292" s="7"/>
       <c r="P292" s="8"/>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A293" s="7">
         <v>395</v>
       </c>
@@ -9306,7 +9334,7 @@
       <c r="O293" s="7"/>
       <c r="P293" s="8"/>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A294" s="7">
         <v>235</v>
       </c>
@@ -9334,7 +9362,7 @@
       <c r="O294" s="7"/>
       <c r="P294" s="8"/>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A295" s="7">
         <v>69</v>
       </c>
@@ -9362,7 +9390,7 @@
       <c r="O295" s="7"/>
       <c r="P295" s="8"/>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A296" s="7">
         <v>165</v>
       </c>
@@ -9390,7 +9418,7 @@
       <c r="O296" s="7"/>
       <c r="P296" s="8"/>
     </row>
-    <row r="297" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="7">
         <v>105</v>
       </c>
@@ -9418,7 +9446,7 @@
       <c r="O297" s="7"/>
       <c r="P297" s="8"/>
     </row>
-    <row r="298" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>0</v>
       </c>
@@ -9467,8 +9495,11 @@
       <c r="P298" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q298">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A299" s="7">
         <v>250</v>
       </c>
@@ -9496,7 +9527,7 @@
       <c r="O299" s="7"/>
       <c r="P299" s="8"/>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A300" s="7">
         <v>191</v>
       </c>
@@ -9524,7 +9555,7 @@
       <c r="O300" s="7"/>
       <c r="P300" s="8"/>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A301" s="7">
         <v>271</v>
       </c>
@@ -9554,7 +9585,7 @@
       <c r="O301" s="7"/>
       <c r="P301" s="8"/>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A302" s="7">
         <v>287</v>
       </c>
@@ -9582,7 +9613,7 @@
       <c r="O302" s="7"/>
       <c r="P302" s="8"/>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A303" s="7">
         <v>371</v>
       </c>
@@ -9610,7 +9641,7 @@
       <c r="O303" s="7"/>
       <c r="P303" s="8"/>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A304" s="7">
         <v>296</v>
       </c>
@@ -10087,7 +10118,7 @@
       <c r="O320" s="7"/>
       <c r="P320" s="8"/>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A321" s="7">
         <v>50</v>
       </c>
@@ -10115,7 +10146,7 @@
       <c r="O321" s="7"/>
       <c r="P321" s="8"/>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A322" s="7">
         <v>334</v>
       </c>
@@ -10143,7 +10174,7 @@
       <c r="O322" s="7"/>
       <c r="P322" s="8"/>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A323" s="7">
         <v>400</v>
       </c>
@@ -10171,7 +10202,7 @@
       <c r="O323" s="7"/>
       <c r="P323" s="8"/>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A324" s="7">
         <v>342</v>
       </c>
@@ -10199,7 +10230,7 @@
       <c r="O324" s="7"/>
       <c r="P324" s="8"/>
     </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A325" s="7">
         <v>6</v>
       </c>
@@ -10229,7 +10260,7 @@
       <c r="O325" s="7"/>
       <c r="P325" s="8"/>
     </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A326" s="7">
         <v>120</v>
       </c>
@@ -10257,7 +10288,7 @@
       <c r="O326" s="7"/>
       <c r="P326" s="8"/>
     </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A327" s="7">
         <v>128</v>
       </c>
@@ -10285,7 +10316,7 @@
       <c r="O327" s="7"/>
       <c r="P327" s="8"/>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A328" s="7">
         <v>350</v>
       </c>
@@ -10313,7 +10344,7 @@
       <c r="O328" s="7"/>
       <c r="P328" s="8"/>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A329" s="7">
         <v>104</v>
       </c>
@@ -10341,7 +10372,7 @@
       <c r="O329" s="7"/>
       <c r="P329" s="8"/>
     </row>
-    <row r="330" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A330" s="7">
         <v>113</v>
       </c>
@@ -10369,7 +10400,7 @@
       <c r="O330" s="7"/>
       <c r="P330" s="8"/>
     </row>
-    <row r="331" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>0</v>
       </c>
@@ -10418,8 +10449,11 @@
       <c r="P331" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q331">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="332" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A332" s="7">
         <v>17</v>
       </c>
@@ -10447,7 +10481,7 @@
       <c r="O332" s="7"/>
       <c r="P332" s="8"/>
     </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A333" s="7">
         <v>137</v>
       </c>
@@ -10475,7 +10509,7 @@
       <c r="O333" s="7"/>
       <c r="P333" s="8"/>
     </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A334" s="7">
         <v>2</v>
       </c>
@@ -10503,7 +10537,7 @@
       <c r="O334" s="7"/>
       <c r="P334" s="8"/>
     </row>
-    <row r="335" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A335" s="7">
         <v>109</v>
       </c>
@@ -10531,7 +10565,7 @@
       <c r="O335" s="7"/>
       <c r="P335" s="8"/>
     </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A336" s="7">
         <v>230</v>
       </c>
@@ -11012,7 +11046,7 @@
       <c r="O352" s="7"/>
       <c r="P352" s="8"/>
     </row>
-    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A353" s="7">
         <v>276</v>
       </c>
@@ -11040,7 +11074,7 @@
       <c r="O353" s="7"/>
       <c r="P353" s="8"/>
     </row>
-    <row r="354" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A354" s="7">
         <v>309</v>
       </c>
@@ -11068,7 +11102,7 @@
       <c r="O354" s="7"/>
       <c r="P354" s="8"/>
     </row>
-    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A355" s="7">
         <v>325</v>
       </c>
@@ -11096,7 +11130,7 @@
       <c r="O355" s="7"/>
       <c r="P355" s="8"/>
     </row>
-    <row r="356" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A356" s="7">
         <v>203</v>
       </c>
@@ -11124,7 +11158,7 @@
       <c r="O356" s="7"/>
       <c r="P356" s="8"/>
     </row>
-    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A357" s="7">
         <v>168</v>
       </c>
@@ -11152,7 +11186,7 @@
       <c r="O357" s="7"/>
       <c r="P357" s="8"/>
     </row>
-    <row r="358" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A358" s="7">
         <v>87</v>
       </c>
@@ -11182,7 +11216,7 @@
       <c r="O358" s="7"/>
       <c r="P358" s="8"/>
     </row>
-    <row r="359" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A359" s="7">
         <v>219</v>
       </c>
@@ -11212,7 +11246,7 @@
       <c r="O359" s="7"/>
       <c r="P359" s="8"/>
     </row>
-    <row r="360" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A360" s="7">
         <v>212</v>
       </c>
@@ -11240,7 +11274,7 @@
       <c r="O360" s="7"/>
       <c r="P360" s="8"/>
     </row>
-    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A361" s="7">
         <v>153</v>
       </c>
@@ -11268,7 +11302,7 @@
       <c r="O361" s="7"/>
       <c r="P361" s="8"/>
     </row>
-    <row r="362" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A362" s="7">
         <v>363</v>
       </c>
@@ -11296,7 +11330,7 @@
       <c r="O362" s="7"/>
       <c r="P362" s="8"/>
     </row>
-    <row r="363" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A363" s="7">
         <v>67</v>
       </c>
@@ -11324,7 +11358,7 @@
       <c r="O363" s="7"/>
       <c r="P363" s="8"/>
     </row>
-    <row r="364" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>0</v>
       </c>
@@ -11373,8 +11407,11 @@
       <c r="P364" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q364">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="365" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A365" s="7">
         <v>374</v>
       </c>
@@ -11402,7 +11439,7 @@
       <c r="O365" s="7"/>
       <c r="P365" s="8"/>
     </row>
-    <row r="366" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A366" s="7">
         <v>234</v>
       </c>
@@ -11430,7 +11467,7 @@
       <c r="O366" s="7"/>
       <c r="P366" s="8"/>
     </row>
-    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A367" s="7">
         <v>281</v>
       </c>
@@ -11458,7 +11495,7 @@
       <c r="O367" s="7"/>
       <c r="P367" s="8"/>
     </row>
-    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A368" s="7">
         <v>243</v>
       </c>
@@ -11939,7 +11976,7 @@
       <c r="O384" s="7"/>
       <c r="P384" s="8"/>
     </row>
-    <row r="385" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A385" s="7">
         <v>25</v>
       </c>
@@ -11967,7 +12004,7 @@
       <c r="O385" s="7"/>
       <c r="P385" s="8"/>
     </row>
-    <row r="386" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A386" s="7">
         <v>148</v>
       </c>
@@ -11995,7 +12032,7 @@
       <c r="O386" s="7"/>
       <c r="P386" s="8"/>
     </row>
-    <row r="387" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A387" s="7">
         <v>183</v>
       </c>
@@ -12023,7 +12060,7 @@
       <c r="O387" s="7"/>
       <c r="P387" s="8"/>
     </row>
-    <row r="388" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A388" s="7">
         <v>354</v>
       </c>
@@ -12051,7 +12088,7 @@
       <c r="O388" s="7"/>
       <c r="P388" s="8"/>
     </row>
-    <row r="389" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A389" s="7">
         <v>266</v>
       </c>
@@ -12081,7 +12118,7 @@
       <c r="O389" s="7"/>
       <c r="P389" s="8"/>
     </row>
-    <row r="390" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A390" s="7">
         <v>44</v>
       </c>
@@ -12109,7 +12146,7 @@
       <c r="O390" s="7"/>
       <c r="P390" s="8"/>
     </row>
-    <row r="391" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A391" s="7">
         <v>152</v>
       </c>
@@ -12137,7 +12174,7 @@
       <c r="O391" s="7"/>
       <c r="P391" s="8"/>
     </row>
-    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A392" s="7">
         <v>305</v>
       </c>
@@ -12165,7 +12202,7 @@
       <c r="O392" s="7"/>
       <c r="P392" s="8"/>
     </row>
-    <row r="393" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A393" s="7">
         <v>291</v>
       </c>
@@ -12195,7 +12232,7 @@
       <c r="O393" s="7"/>
       <c r="P393" s="8"/>
     </row>
-    <row r="394" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A394" s="7">
         <v>297</v>
       </c>
@@ -12223,7 +12260,7 @@
       <c r="O394" s="7"/>
       <c r="P394" s="8"/>
     </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A395" s="7">
         <v>134</v>
       </c>
@@ -12251,7 +12288,7 @@
       <c r="O395" s="7"/>
       <c r="P395" s="8"/>
     </row>
-    <row r="396" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A396" s="7">
         <v>118</v>
       </c>
@@ -12279,7 +12316,7 @@
       <c r="O396" s="7"/>
       <c r="P396" s="8"/>
     </row>
-    <row r="397" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>0</v>
       </c>
@@ -12328,8 +12365,11 @@
       <c r="P397" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="398" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q397">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="398" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A398" s="7">
         <v>166</v>
       </c>
@@ -12357,7 +12397,7 @@
       <c r="O398" s="7"/>
       <c r="P398" s="8"/>
     </row>
-    <row r="399" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A399" s="7">
         <v>331</v>
       </c>
@@ -12385,7 +12425,7 @@
       <c r="O399" s="7"/>
       <c r="P399" s="8"/>
     </row>
-    <row r="400" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A400" s="7">
         <v>252</v>
       </c>

</xml_diff>

<commit_message>
End of the day, remaining changes.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/flight_trials_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C26E6B-89BC-C742-B3EA-3C1F7B0AE786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36690B9-CE65-4747-A9BA-D818E8C61834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="500" windowWidth="26880" windowHeight="16640" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
+    <workbookView xWindow="1920" yWindow="500" windowWidth="26880" windowHeight="16640" xr2:uid="{7B0EB56A-DD96-9F4A-80C4-FF3A8A73FC6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322886B1-E7FD-B647-8810-B789824E1075}">
   <dimension ref="A1:Q445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="125" workbookViewId="0">
-      <selection activeCell="Q198" sqref="Q198"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6396,7 +6396,9 @@
       <c r="A193" s="7">
         <v>399</v>
       </c>
-      <c r="B193" s="7"/>
+      <c r="B193" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>

</xml_diff>